<commit_message>
/honorari route adds form input data to .xlsx file and downloads it afterwards.
</commit_message>
<xml_diff>
--- a/static/files/tablica-honorari.xlsx
+++ b/static/files/tablica-honorari.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PycharmProjects\AdministrationManager\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13C3B44-8E2E-4CF9-9F09-F2B11E9A2A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F658DA9-F4A6-4950-A7E2-557A9886013D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="1800" windowWidth="22605" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5565" yWindow="1590" windowWidth="22605" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -253,14 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -269,14 +261,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,7 +600,7 @@
   <dimension ref="A3:AC22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:O24"/>
+      <selection activeCell="AB12" sqref="A12:AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,81 +611,81 @@
     <col min="4" max="27" width="3.140625" style="1" customWidth="1"/>
     <col min="28" max="28" width="5" style="1" customWidth="1"/>
     <col min="29" max="29" width="4" style="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="1"/>
+    <col min="30" max="33" width="9.140625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="J3" s="15" t="s">
+      <c r="B3" s="13"/>
+      <c r="J3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="G4" s="16" t="s">
+      <c r="B4" s="13"/>
+      <c r="G4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="3"/>
+      <c r="B5" s="13"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="F7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
     </row>
     <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -694,41 +694,41 @@
       <c r="C9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="7" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AC9" s="8"/>
+      <c r="AC9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -753,41 +753,41 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="10"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="4" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="8"/>
     </row>
     <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -817,8 +817,8 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="6"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="16"/>
     </row>
     <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -848,8 +848,8 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="6"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="16"/>
     </row>
     <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -879,8 +879,8 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="6"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="16"/>
     </row>
     <row r="15" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -910,8 +910,8 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="6"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="16"/>
     </row>
     <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -941,61 +941,70 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="6"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="16"/>
     </row>
     <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="6"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="16"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="X22" s="3" t="s">
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="X22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="X22:AC22"/>
+    <mergeCell ref="B17:AA17"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AB9:AC11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="J3:O3"/>
@@ -1010,17 +1019,8 @@
     <mergeCell ref="D9:AA9"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="X22:AC22"/>
-    <mergeCell ref="B17:AA17"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB15:AC15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated templates so that custom user settings are added.
</commit_message>
<xml_diff>
--- a/static/files/tablica-honorari.xlsx
+++ b/static/files/tablica-honorari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PycharmProjects\AdministrationManager\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F658DA9-F4A6-4950-A7E2-557A9886013D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6085F85-0E5C-442E-BF55-94FE32E17747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5565" yWindow="1590" windowWidth="22605" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,27 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>SREDNJA ŠKOLA ILOK</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>TABLICA</t>
   </si>
   <si>
-    <t>Matije Gupca 168</t>
-  </si>
-  <si>
     <t>za održane honorarne sate u mjesecu</t>
   </si>
   <si>
-    <t>32236 Ilok</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prezime i ime učitelja - nastavnika: </t>
-  </si>
-  <si>
-    <t>___________________________________________________</t>
   </si>
   <si>
     <t>PREDMET</t>
@@ -75,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +98,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -253,6 +250,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -261,27 +266,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,7 +600,7 @@
   <dimension ref="A3:AC22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="A12:AC12"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,119 +616,111 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3"/>
+      <c r="J3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="3"/>
+      <c r="G4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-    </row>
-    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="G4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="13"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="3"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+    </row>
+    <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-    </row>
-    <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC9" s="4"/>
+      <c r="AC9" s="8"/>
     </row>
     <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -753,41 +745,41 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="6"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="10"/>
     </row>
     <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="8"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="12"/>
     </row>
     <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -817,8 +809,8 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="16"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="6"/>
     </row>
     <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -848,8 +840,8 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="16"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="6"/>
     </row>
     <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -879,8 +871,8 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="16"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="6"/>
     </row>
     <row r="15" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -910,8 +902,8 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="16"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="6"/>
     </row>
     <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -941,70 +933,61 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="16"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="6"/>
     </row>
     <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="16"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="6"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="X22" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
+      <c r="J22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="X22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="X22:AC22"/>
-    <mergeCell ref="B17:AA17"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AB9:AC11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="J3:O3"/>
@@ -1019,8 +1002,17 @@
     <mergeCell ref="D9:AA9"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="B9:B11"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="X22:AC22"/>
+    <mergeCell ref="B17:AA17"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB15:AC15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed get_row() function in honorarium_excel.py and updated .xlsx template to show previous month, instead of current.
</commit_message>
<xml_diff>
--- a/static/files/tablica-honorari.xlsx
+++ b/static/files/tablica-honorari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PycharmProjects\AdministrationManager\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\PycharmProjects\AdministrationManager\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6085F85-0E5C-442E-BF55-94FE32E17747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378D4C4F-CD98-4F44-860A-FCB6E8A7AEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="1590" windowWidth="22605" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -250,14 +250,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -266,22 +258,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,7 +600,7 @@
   <dimension ref="A3:AC22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="K5" sqref="K5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,111 +616,113 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="3"/>
-      <c r="J3" s="15" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="J3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="3"/>
-      <c r="G4" s="16" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="G4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="3"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="3"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
     </row>
     <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="7" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AC9" s="8"/>
+      <c r="AC9" s="4"/>
     </row>
     <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -745,41 +747,41 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="10"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="6"/>
     </row>
     <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="4" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="12"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="8"/>
     </row>
     <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -809,8 +811,8 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="6"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="16"/>
     </row>
     <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -840,8 +842,8 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="6"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="16"/>
     </row>
     <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -871,8 +873,8 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
-      <c r="AB14" s="7"/>
-      <c r="AC14" s="6"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="16"/>
     </row>
     <row r="15" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -902,8 +904,8 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="6"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="16"/>
     </row>
     <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -933,66 +935,74 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
-      <c r="AB16" s="7"/>
-      <c r="AC16" s="6"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="16"/>
     </row>
     <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="5"/>
-      <c r="W17" s="5"/>
-      <c r="X17" s="5"/>
-      <c r="Y17" s="5"/>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="6"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="16"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="X22" s="3" t="s">
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="X22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="X22:AC22"/>
+    <mergeCell ref="B17:AA17"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AB9:AC11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="J3:O3"/>
     <mergeCell ref="G4:R4"/>
-    <mergeCell ref="L5:M5"/>
     <mergeCell ref="D11:AA11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
@@ -1002,15 +1012,7 @@
     <mergeCell ref="D9:AA9"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="B9:B11"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="X22:AC22"/>
-    <mergeCell ref="B17:AA17"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="K5:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed unnecessary files and fixed honorarium_excel.py as the file in memory was not being downloaded properly
</commit_message>
<xml_diff>
--- a/static/files/tablica-honorari.xlsx
+++ b/static/files/tablica-honorari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korisnik\PycharmProjects\AdministrationManager\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PycharmProjects\AdministrationManager\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378D4C4F-CD98-4F44-860A-FCB6E8A7AEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F2CE17-64C2-4915-BCA7-60183EF9FDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="1470" windowWidth="22605" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TABLICA</t>
   </si>
   <si>
     <t>za održane honorarne sate u mjesecu</t>
+  </si>
+  <si>
+    <t>02/2023</t>
   </si>
   <si>
     <t xml:space="preserve">Prezime i ime učitelja - nastavnika: </t>
@@ -244,12 +247,20 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -258,22 +269,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,405 +603,398 @@
   <dimension ref="A3:AC22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:N5"/>
+      <selection activeCell="F7" sqref="F7:V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="27" width="3.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="5" style="1" customWidth="1"/>
-    <col min="29" max="29" width="4" style="1" customWidth="1"/>
-    <col min="30" max="33" width="9.140625" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="38.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" style="2" customWidth="1"/>
+    <col min="4" max="27" width="3.140625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="5" style="2" customWidth="1"/>
+    <col min="29" max="29" width="4" style="2" customWidth="1"/>
+    <col min="30" max="34" width="9.140625" style="2" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="13"/>
-      <c r="J3" s="12" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3"/>
+      <c r="J3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13"/>
-      <c r="G4" s="14" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="3"/>
+      <c r="G4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
     </row>
     <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>3</v>
+      <c r="A9" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AC9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC9" s="8"/>
     </row>
     <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="6"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="10"/>
     </row>
     <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="8"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="12"/>
     </row>
     <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="16"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="6"/>
     </row>
     <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="16"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="6"/>
     </row>
     <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="16"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="6"/>
     </row>
     <row r="15" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="16"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="6"/>
     </row>
     <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="16"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="6"/>
     </row>
     <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="16"/>
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="6"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J22" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="X22" s="13" t="s">
+      <c r="J22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13"/>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="X22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AC22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="X22:AC22"/>
-    <mergeCell ref="B17:AA17"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB13:AC13"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AB16:AC16"/>
-    <mergeCell ref="AB17:AC17"/>
-    <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="AB9:AC11"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="J3:O3"/>
@@ -1013,8 +1009,17 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="K5:N5"/>
+    <mergeCell ref="J22:N22"/>
+    <mergeCell ref="X22:AC22"/>
+    <mergeCell ref="B17:AA17"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AB17:AC17"/>
+    <mergeCell ref="AB15:AC15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>